<commit_message>
feat(data): support price and return input types, update docs
Adds CLI support for both price and single-period return data as input,
controlled by the --input-type argument. Updates all docstrings to
reStructuredText and clarifies requirements for input data, including
the need for true single-period returns (not annualized rates) when
using return input. Improves documentation and code clarity for both
modes of operation.
</commit_message>
<xml_diff>
--- a/data/EONIARATE.xlsx
+++ b/data/EONIARATE.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="EONIARATE" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="EONIARATE(1)" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve">DATE</t>
+    <t xml:space="preserve">Date</t>
   </si>
   <si>
     <t xml:space="preserve">EONIARATE</t>
@@ -244,14 +244,16 @@
   </sheetPr>
   <dimension ref="A1:B5999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>